<commit_message>
updated materials for Balas following his comments
</commit_message>
<xml_diff>
--- a/measures/3 translation and stimuli selection/2 sites/Balas & Sarzynska/translation/Polish/awareness_1.xlsx
+++ b/measures/3 translation and stimuli selection/2 sites/Balas & Sarzynska/translation/Polish/awareness_1.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tmoranyo\Documents\GitHub\RRR_fazio-olson2001-local\tal-creation\4 site-specific measures for data collection\Balas &amp; Sarzynska\text\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4335" yWindow="5415" windowWidth="26820" windowHeight="17040"/>
+    <workbookView xWindow="4335" yWindow="5415" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="instructions" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -42,7 +37,7 @@
   </si>
   <si>
     <t>Czy zauważyłeś coś charakterstycznego w słowach i obrazach, które pojawiały się z określonymi postaciami z kreskówek?
-Wpisz swoją odpowiedź za pomocą klawiatury, która pojawi się poniżej.
+Wpisz swoją odpowiedź za pomocą klawiatury.
 Naciśnij Enter by przejść do następnego pytania.
 Twoja odpowiedź musi mieć minimum 20 znaków.</t>
   </si>
@@ -50,8 +45,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="18">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -553,48 +548,48 @@
     </xf>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="20% - akcent 1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - akcent 2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - akcent 3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - akcent 4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - akcent 5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - akcent 6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - akcent 1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - akcent 2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - akcent 3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - akcent 4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - akcent 5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - akcent 6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - akcent 1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - akcent 2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - akcent 3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - akcent 4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - akcent 5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - akcent 6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Akcent 1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Akcent 2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Akcent 3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Akcent 4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Akcent 5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Akcent 6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Dane wejściowe" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Dane wyjściowe" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Dobre" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Komórka połączona" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Komórka zaznaczona" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Nagłówek 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Nagłówek 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Nagłówek 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Nagłówek 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Neutralne" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
+    <cellStyle name="Obliczenia" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Suma" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Tekst objaśnienia" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Tekst ostrzeżenia" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Tytuł" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Uwaga" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Złe" xfId="7" builtinId="27" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -898,47 +893,46 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="89.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="126.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" ht="126.95" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="126" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" ht="126" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="117" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" ht="117" customHeight="1">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>